<commit_message>
Correct metadata in excel files for repository migration tests.
</commit_message>
<xml_diff>
--- a/opengever/bundle/tests/assets/os_migration/os_test_branch_and_leaf_creation.xlsx
+++ b/opengever/bundle/tests/assets/os_migration/os_test_branch_and_leaf_creation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Work/development/opengever.core/opengever/bundle/tests/assets/os_migration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklausjohner/Work/development/opengever.core2/opengever/bundle/tests/assets/os_migration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0490BE-F264-BB42-9421-8F0B4178B13B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52DDB4B-B441-4C47-94D6-05E7FC6DA480}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="7660" windowWidth="25920" windowHeight="10340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1940" yWindow="9880" windowWidth="25920" windowHeight="10340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordnungssystem" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
   <si>
     <t>reference_number</t>
   </si>
@@ -873,7 +873,7 @@
     <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1097,6 +1097,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1642,9 +1645,9 @@
   <sheetPr codeName="Blatt1"/>
   <dimension ref="A1:AC526"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2034,19 +2037,21 @@
       </c>
       <c r="J7" s="56"/>
       <c r="K7" s="56"/>
-      <c r="L7" s="13" t="s">
+      <c r="L7" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="M7" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="N7" s="13">
-        <v>20</v>
-      </c>
-      <c r="P7" s="13" t="s">
+      <c r="N7" s="77">
+        <v>5</v>
+      </c>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="R7" s="13">
+      <c r="Q7" s="77"/>
+      <c r="R7" s="77">
         <v>30</v>
       </c>
       <c r="S7" s="14"/>
@@ -2085,21 +2090,13 @@
       <c r="I8" s="11"/>
       <c r="J8" s="56"/>
       <c r="K8" s="56"/>
-      <c r="L8" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="N8" s="13">
-        <v>20</v>
-      </c>
-      <c r="P8" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="R8" s="13">
-        <v>30</v>
-      </c>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="77"/>
+      <c r="P8" s="77"/>
+      <c r="Q8" s="77"/>
+      <c r="R8" s="77"/>
       <c r="S8" s="14"/>
       <c r="T8" s="12"/>
       <c r="U8" s="12"/>
@@ -2132,6 +2129,23 @@
       <c r="I9" s="11"/>
       <c r="J9" s="56"/>
       <c r="K9" s="56"/>
+      <c r="L9" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9" s="77">
+        <v>5</v>
+      </c>
+      <c r="O9" s="77"/>
+      <c r="P9" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="77"/>
+      <c r="R9" s="77">
+        <v>30</v>
+      </c>
       <c r="S9" s="14"/>
       <c r="T9" s="12"/>
       <c r="U9" s="12"/>
@@ -2163,6 +2177,23 @@
       <c r="I10" s="74"/>
       <c r="J10" s="74"/>
       <c r="K10" s="75"/>
+      <c r="L10" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" s="77">
+        <v>5</v>
+      </c>
+      <c r="O10" s="77"/>
+      <c r="P10" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q10" s="77"/>
+      <c r="R10" s="77">
+        <v>30</v>
+      </c>
       <c r="S10" s="71"/>
       <c r="T10" s="72"/>
       <c r="U10" s="72"/>
@@ -2275,19 +2306,21 @@
       </c>
       <c r="J13" s="56"/>
       <c r="K13" s="56"/>
-      <c r="L13" s="13" t="s">
+      <c r="L13" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="13" t="s">
+      <c r="M13" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="N13" s="13">
-        <v>20</v>
-      </c>
-      <c r="P13" s="13" t="s">
+      <c r="N13" s="77">
+        <v>5</v>
+      </c>
+      <c r="O13" s="77"/>
+      <c r="P13" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="R13" s="13">
+      <c r="Q13" s="77"/>
+      <c r="R13" s="77">
         <v>30</v>
       </c>
       <c r="S13" s="14"/>
@@ -15889,7 +15922,7 @@
           <x14:formula1>
             <xm:f>Wertebereich!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>M7:M9 M11:M1048576</xm:sqref>
+          <xm:sqref>M11:M12 M14:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
@@ -15901,25 +15934,25 @@
           <x14:formula1>
             <xm:f>Wertebereich!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>L7:L9 L11:L1048576</xm:sqref>
+          <xm:sqref>L11:L12 L14:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>Wertebereich!$J$2:$J$7</xm:f>
           </x14:formula1>
-          <xm:sqref>P7:P9 P11:P1048576</xm:sqref>
+          <xm:sqref>P11:P12 P14:P1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>Wertebereich!$H$2:$H$6</xm:f>
           </x14:formula1>
-          <xm:sqref>N7:N9 N11:N1048576</xm:sqref>
+          <xm:sqref>N11:N12 N14:N1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>Wertebereich!$L$2:$L$4</xm:f>
           </x14:formula1>
-          <xm:sqref>R7:R9 R11:R1048576</xm:sqref>
+          <xm:sqref>R11:R12 R14:R1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -16108,27 +16141,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <oc_termin_lookup_helper xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
-    <oc_traktandum_lookup xmlns="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
-    <oc_termin_lookup xmlns="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
-    <oc_document_is_common xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
-    <oc_traktandum_lookup_helper xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100440900994F0F214B9EC76DEC64CCCEC3" ma:contentTypeVersion="" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="3c93ed4d6daf505d37aacf3e1bef2534">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="96CA5592-7E49-4C69-936A-77E0F19F316B" xmlns:ns3="82675a1d-2274-46ff-95b6-7e628f04e7b8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c3cc4f1e90dff483e4da45e10a5d6cb" ns2:_="" ns3:_="">
     <xsd:import namespace="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
@@ -16319,26 +16331,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63B1394A-812F-4D99-A0FC-B41B7F31C120}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="82675a1d-2274-46ff-95b6-7e628f04e7b8"/>
-    <ds:schemaRef ds:uri="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B73656-B986-42B5-A6F0-2CB7C4F8F507}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <oc_termin_lookup_helper xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
+    <oc_traktandum_lookup xmlns="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
+    <oc_termin_lookup xmlns="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
+    <oc_document_is_common xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
+    <oc_traktandum_lookup_helper xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37806679-E8E8-4A87-9E25-D47F01162BB9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16355,4 +16369,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B73656-B986-42B5-A6F0-2CB7C4F8F507}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63B1394A-812F-4D99-A0FC-B41B7F31C120}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="82675a1d-2274-46ff-95b6-7e628f04e7b8"/>
+    <ds:schemaRef ds:uri="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adapt tests to handling of metadata and permissions.
</commit_message>
<xml_diff>
--- a/opengever/bundle/tests/assets/os_migration/os_test_branch_and_leaf_creation.xlsx
+++ b/opengever/bundle/tests/assets/os_migration/os_test_branch_and_leaf_creation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklausjohner/Work/development/opengever.core2/opengever/bundle/tests/assets/os_migration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklausjohner/Work/development/opengever.core/opengever/bundle/tests/assets/os_migration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52DDB4B-B441-4C47-94D6-05E7FC6DA480}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE10269-047D-0342-8784-5D82A7C9EF84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="9880" windowWidth="25920" windowHeight="10340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="2140" windowWidth="34680" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordnungssystem" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="109">
   <si>
     <t>reference_number</t>
   </si>
@@ -482,6 +482,12 @@
   </si>
   <si>
     <t>Alles zum Thema Führung.</t>
+  </si>
+  <si>
+    <t>faivel.fruhling</t>
+  </si>
+  <si>
+    <t>jurgen.fischer</t>
   </si>
 </sst>
 </file>
@@ -1647,7 +1653,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U8" sqref="U8"/>
+      <selection pane="bottomLeft" activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2064,7 +2070,9 @@
       <c r="Z7" s="15"/>
       <c r="AA7" s="15"/>
       <c r="AB7" s="15"/>
-      <c r="AC7" s="15"/>
+      <c r="AC7" s="15" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="8" spans="1:29" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="29"/>
@@ -2103,10 +2111,6 @@
       <c r="V8" s="12"/>
       <c r="W8" s="15"/>
       <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="15"/>
-      <c r="AB8" s="15"/>
       <c r="AC8" s="15"/>
     </row>
     <row r="9" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.15">
@@ -2152,10 +2156,14 @@
       <c r="V9" s="12"/>
       <c r="W9" s="15"/>
       <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
+      <c r="Y9" s="15" t="s">
+        <v>108</v>
+      </c>
       <c r="Z9" s="15"/>
       <c r="AA9" s="15"/>
-      <c r="AB9" s="15"/>
+      <c r="AB9" s="15" t="s">
+        <v>108</v>
+      </c>
       <c r="AC9" s="15"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.15">
@@ -16332,15 +16340,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <oc_termin_lookup_helper xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
@@ -16350,6 +16349,15 @@
     <oc_traktandum_lookup_helper xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16372,14 +16380,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B73656-B986-42B5-A6F0-2CB7C4F8F507}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63B1394A-812F-4D99-A0FC-B41B7F31C120}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -16388,4 +16388,12 @@
     <ds:schemaRef ds:uri="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B73656-B986-42B5-A6F0-2CB7C4F8F507}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>